<commit_message>
add modules to programs
</commit_message>
<xml_diff>
--- a/public/data/programs.xlsx
+++ b/public/data/programs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="117">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Year/Level</t>
   </si>
   <si>
+    <t xml:space="preserve">Program Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Help Desk &amp; Project Management</t>
   </si>
   <si>
@@ -58,78 +61,150 @@
     <t xml:space="preserve">Months</t>
   </si>
   <si>
+    <t xml:space="preserve">STC100</t>
+  </si>
+  <si>
     <t xml:space="preserve">Machine Learning - Beginner</t>
   </si>
   <si>
+    <t xml:space="preserve">STC101</t>
+  </si>
+  <si>
     <t xml:space="preserve">It@Workplace Advanced</t>
   </si>
   <si>
+    <t xml:space="preserve">STC102</t>
+  </si>
+  <si>
     <t xml:space="preserve">Social Media Marketing</t>
   </si>
   <si>
+    <t xml:space="preserve">STC103</t>
+  </si>
+  <si>
     <t xml:space="preserve">It@Workplace Primer</t>
   </si>
   <si>
+    <t xml:space="preserve">STC104</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cyber Security- Ncc</t>
   </si>
   <si>
+    <t xml:space="preserve">STC105</t>
+  </si>
+  <si>
     <t xml:space="preserve">Intro. To Blockchain</t>
   </si>
   <si>
+    <t xml:space="preserve">STC106</t>
+  </si>
+  <si>
     <t xml:space="preserve">HTML 5 &amp; CSS3</t>
   </si>
   <si>
+    <t xml:space="preserve">STC107</t>
+  </si>
+  <si>
     <t xml:space="preserve">R Tools For Statistics</t>
   </si>
   <si>
     <t xml:space="preserve">Weeks</t>
   </si>
   <si>
+    <t xml:space="preserve">STC108</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aws Certification </t>
   </si>
   <si>
+    <t xml:space="preserve">STC109</t>
+  </si>
+  <si>
     <t xml:space="preserve">Robotics</t>
   </si>
   <si>
+    <t xml:space="preserve">STC110</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ms Power Bi</t>
   </si>
   <si>
+    <t xml:space="preserve">STC111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ms Excel 2019</t>
   </si>
   <si>
+    <t xml:space="preserve">STC112</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tally - Basic</t>
   </si>
   <si>
+    <t xml:space="preserve">STC113</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tally - Advance </t>
   </si>
   <si>
+    <t xml:space="preserve">STC114</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cloud Computing </t>
   </si>
   <si>
+    <t xml:space="preserve">STC115</t>
+  </si>
+  <si>
     <t xml:space="preserve">Python</t>
   </si>
   <si>
+    <t xml:space="preserve">STC116</t>
+  </si>
+  <si>
     <t xml:space="preserve">Excel + Adv Excel</t>
   </si>
   <si>
+    <t xml:space="preserve">STC117</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comptia n+</t>
   </si>
   <si>
+    <t xml:space="preserve">STC118</t>
+  </si>
+  <si>
     <t xml:space="preserve">Autocad </t>
   </si>
   <si>
+    <t xml:space="preserve">STC119</t>
+  </si>
+  <si>
     <t xml:space="preserve">Accounting with I.T</t>
   </si>
   <si>
+    <t xml:space="preserve">STC120</t>
+  </si>
+  <si>
     <t xml:space="preserve">Big Data Analytics </t>
   </si>
   <si>
+    <t xml:space="preserve">STC121</t>
+  </si>
+  <si>
     <t xml:space="preserve">Artificial Intelligence </t>
   </si>
   <si>
+    <t xml:space="preserve">STC122</t>
+  </si>
+  <si>
     <t xml:space="preserve">C++</t>
   </si>
   <si>
+    <t xml:space="preserve">STC123</t>
+  </si>
+  <si>
     <t xml:space="preserve">System Engineering</t>
   </si>
   <si>
@@ -139,55 +214,166 @@
     <t xml:space="preserve">Level 1</t>
   </si>
   <si>
+    <t xml:space="preserve">PD100</t>
+  </si>
+  <si>
     <t xml:space="preserve">Software Engineering</t>
   </si>
   <si>
+    <t xml:space="preserve">PD101</t>
+  </si>
+  <si>
     <t xml:space="preserve">Database Technology</t>
   </si>
   <si>
+    <t xml:space="preserve">PD102</t>
+  </si>
+  <si>
     <t xml:space="preserve">Digital Marketing</t>
   </si>
   <si>
+    <t xml:space="preserve">PD103</t>
+  </si>
+  <si>
     <t xml:space="preserve">Graphic &amp; Web Designing</t>
   </si>
   <si>
+    <t xml:space="preserve">PD104</t>
+  </si>
+  <si>
     <t xml:space="preserve">Year 1</t>
   </si>
   <si>
+    <t xml:space="preserve">PD105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD109</t>
+  </si>
+  <si>
     <t xml:space="preserve">Year 2</t>
   </si>
   <si>
+    <t xml:space="preserve">PD110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD114</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level 2</t>
   </si>
   <si>
+    <t xml:space="preserve">PD115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD119</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level 3</t>
   </si>
   <si>
+    <t xml:space="preserve">PD120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD124</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level 4</t>
   </si>
   <si>
+    <t xml:space="preserve">PD125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD129</t>
+  </si>
+  <si>
     <t xml:space="preserve">L3DC - Diploma in Computing</t>
   </si>
   <si>
     <t xml:space="preserve">Degree</t>
   </si>
   <si>
+    <t xml:space="preserve">D100</t>
+  </si>
+  <si>
     <t xml:space="preserve">L4DBIT - Diploma in Business Information Technology</t>
   </si>
   <si>
+    <t xml:space="preserve">D101</t>
+  </si>
+  <si>
     <t xml:space="preserve">L5DBIT – Adv. Diploma in Business Information Technology</t>
   </si>
   <si>
+    <t xml:space="preserve">D102</t>
+  </si>
+  <si>
     <t xml:space="preserve">BSc (Hon) Computing</t>
   </si>
   <si>
+    <t xml:space="preserve">D103</t>
+  </si>
+  <si>
     <t xml:space="preserve">BSc (Hon) Information Technology</t>
   </si>
   <si>
+    <t xml:space="preserve">D104</t>
+  </si>
+  <si>
     <t xml:space="preserve">BSc (Hon) Multimedia and Animation Design</t>
   </si>
   <si>
+    <t xml:space="preserve">D105</t>
+  </si>
+  <si>
     <t xml:space="preserve">BSc (Hon) Business Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D106</t>
   </si>
 </sst>
 </file>
@@ -291,17 +477,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G56" activeCellId="0" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.14"/>
   </cols>
@@ -331,19 +517,22 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>2850</v>
@@ -354,19 +543,22 @@
       <c r="G2" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1000</v>
@@ -377,19 +569,22 @@
       <c r="G3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I3" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1900</v>
@@ -400,19 +595,22 @@
       <c r="G4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I4" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1100</v>
@@ -423,19 +621,22 @@
       <c r="G5" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I5" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1350</v>
@@ -446,19 +647,22 @@
       <c r="G6" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I6" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>2650</v>
@@ -469,19 +673,22 @@
       <c r="G7" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I7" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1100</v>
@@ -492,19 +699,22 @@
       <c r="G8" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I8" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>700</v>
@@ -515,19 +725,22 @@
       <c r="G9" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I9" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1650</v>
@@ -538,19 +751,22 @@
       <c r="G10" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I10" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1525</v>
@@ -561,19 +777,22 @@
       <c r="G11" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I11" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1650</v>
@@ -584,19 +803,22 @@
       <c r="G12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I12" s="0" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>2400</v>
@@ -607,19 +829,22 @@
       <c r="G13" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I13" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>625</v>
@@ -630,19 +855,22 @@
       <c r="G14" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I14" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1100</v>
@@ -653,19 +881,22 @@
       <c r="G15" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I15" s="0" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1650</v>
@@ -676,19 +907,22 @@
       <c r="G16" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I16" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1500</v>
@@ -699,19 +933,22 @@
       <c r="G17" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I17" s="0" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1750</v>
@@ -722,19 +959,22 @@
       <c r="G18" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I18" s="0" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1150</v>
@@ -745,19 +985,22 @@
       <c r="G19" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I19" s="0" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>2900</v>
@@ -768,19 +1011,22 @@
       <c r="G20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I20" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1350</v>
@@ -791,19 +1037,22 @@
       <c r="G21" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I21" s="0" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1150</v>
@@ -814,19 +1063,22 @@
       <c r="G22" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I22" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>1650</v>
@@ -837,19 +1089,22 @@
       <c r="G23" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I23" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>1650</v>
@@ -860,19 +1115,22 @@
       <c r="G24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I24" s="0" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1650</v>
@@ -883,19 +1141,22 @@
       <c r="G25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="I25" s="0" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>3218</v>
@@ -907,21 +1168,24 @@
         <v>5</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>3218</v>
@@ -933,21 +1197,24 @@
         <v>5</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>3218</v>
@@ -959,21 +1226,24 @@
         <v>5</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3218</v>
@@ -985,21 +1255,24 @@
         <v>5</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>3218</v>
@@ -1011,21 +1284,24 @@
         <v>5</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>6173</v>
@@ -1037,21 +1313,24 @@
         <v>8</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>42</v>
+        <v>72</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>5781</v>
@@ -1063,21 +1342,24 @@
         <v>8</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>42</v>
+        <v>72</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>5781</v>
@@ -1089,21 +1371,24 @@
         <v>8</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>42</v>
+        <v>72</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>5781</v>
@@ -1115,21 +1400,24 @@
         <v>8</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>42</v>
+        <v>72</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>5781</v>
@@ -1141,21 +1429,24 @@
         <v>8</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>42</v>
+        <v>72</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>6345</v>
@@ -1167,21 +1458,24 @@
         <v>8</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>43</v>
+        <v>78</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>6345</v>
@@ -1193,21 +1487,24 @@
         <v>8</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>43</v>
+        <v>78</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>6345</v>
@@ -1219,21 +1516,24 @@
         <v>8</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>43</v>
+        <v>78</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>6345</v>
@@ -1245,21 +1545,24 @@
         <v>8</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>43</v>
+        <v>78</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>6345</v>
@@ -1271,21 +1574,24 @@
         <v>8</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>43</v>
+        <v>78</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>3457</v>
@@ -1297,21 +1603,24 @@
         <v>5</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>44</v>
+        <v>84</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>3457</v>
@@ -1323,21 +1632,24 @@
         <v>5</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>44</v>
+        <v>84</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>3457</v>
@@ -1349,21 +1661,24 @@
         <v>5</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>44</v>
+        <v>84</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>3457</v>
@@ -1375,21 +1690,24 @@
         <v>5</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>44</v>
+        <v>84</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>3457</v>
@@ -1401,21 +1719,24 @@
         <v>5</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>44</v>
+        <v>84</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>3600</v>
@@ -1427,21 +1748,24 @@
         <v>5</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>45</v>
+        <v>90</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>3600</v>
@@ -1453,21 +1777,24 @@
         <v>5</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>45</v>
+        <v>90</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>3600</v>
@@ -1479,21 +1806,24 @@
         <v>5</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>45</v>
+        <v>90</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>3600</v>
@@ -1505,21 +1835,24 @@
         <v>5</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>45</v>
+        <v>90</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>3600</v>
@@ -1531,21 +1864,24 @@
         <v>5</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>45</v>
+        <v>90</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>3816</v>
@@ -1557,21 +1893,24 @@
         <v>5</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>46</v>
+        <v>96</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>3816</v>
@@ -1583,21 +1922,24 @@
         <v>5</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>46</v>
+        <v>96</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>3816</v>
@@ -1609,21 +1951,24 @@
         <v>5</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>46</v>
+        <v>96</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>3816</v>
@@ -1635,21 +1980,24 @@
         <v>5</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>46</v>
+        <v>96</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>3816</v>
@@ -1661,21 +2009,24 @@
         <v>5</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>46</v>
+        <v>96</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>1836</v>
@@ -1686,19 +2037,22 @@
       <c r="G56" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="I56" s="0" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>2662</v>
@@ -1709,19 +2063,22 @@
       <c r="G57" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="I57" s="0" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>3102</v>
@@ -1732,19 +2089,22 @@
       <c r="G58" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="I58" s="0" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>4885</v>
@@ -1755,19 +2115,22 @@
       <c r="G59" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="I59" s="0" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>2750</v>
@@ -1778,19 +2141,22 @@
       <c r="G60" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="I60" s="0" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>3000</v>
@@ -1801,19 +2167,22 @@
       <c r="G61" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="I61" s="0" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>3000</v>
@@ -1823,6 +2192,9 @@
       </c>
       <c r="G62" s="0" t="n">
         <v>6</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>